<commit_message>
Updated analyses with extended species
</commit_message>
<xml_diff>
--- a/data/codeml/mutation_rate/mutation_rate_analysis_Exo70.xlsx
+++ b/data/codeml/mutation_rate/mutation_rate_analysis_Exo70.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -115,6 +115,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -386,7 +389,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -413,21 +416,21 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-11592.219257000001</v>
+        <v>-13005.275962</v>
       </c>
       <c r="C2">
-        <v>0.21304999999999999</v>
+        <v>0.21745</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
       </c>
       <c r="H2">
         <f>2*(B3-B2)</f>
-        <v>1.7877660000012838</v>
+        <v>3.474819999999454</v>
       </c>
       <c r="I2">
         <f>1-_xlfn.CHISQ.DIST(H2,1,1)</f>
-        <v>0.18119859066948196</v>
+        <v>6.2309500774450521E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -435,20 +438,20 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-11591.325374</v>
+        <v>-13003.538552</v>
       </c>
       <c r="C3">
-        <v>0.21481</v>
+        <v>0.21965000000000001</v>
       </c>
       <c r="D3">
-        <v>9.4159999999999994E-2</v>
+        <v>7.7619999999999995E-2</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
       </c>
       <c r="H3">
         <f>2*(B4-B2)</f>
-        <v>211.5361840000005</v>
+        <v>266.76518399999986</v>
       </c>
       <c r="I3">
         <f>1-_xlfn.CHISQ.DIST(H3,1,1)</f>
@@ -460,24 +463,24 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-11486.451165</v>
+        <v>-12871.89337</v>
       </c>
       <c r="C4">
-        <v>0.1016</v>
+        <v>9.2050000000000007E-2</v>
       </c>
       <c r="D4">
-        <v>0.42304999999999998</v>
+        <v>0.41310000000000002</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
       </c>
       <c r="H4">
         <f>2*(B5-B4)</f>
-        <v>12.019442000000709</v>
+        <v>9.0186839999987569</v>
       </c>
       <c r="I4">
         <f>1-_xlfn.CHISQ.DIST(H4,1,1)</f>
-        <v>5.2648461892956799E-4</v>
+        <v>2.6723372592123429E-3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -485,16 +488,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-11480.441444</v>
+        <v>-12867.384028</v>
       </c>
       <c r="C5">
-        <v>0.13222999999999999</v>
+        <v>0.11772000000000001</v>
       </c>
       <c r="D5">
-        <v>0.42286000000000001</v>
+        <v>0.41298000000000001</v>
       </c>
       <c r="E5">
-        <v>7.8479999999999994E-2</v>
+        <v>7.5029999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>